<commit_message>
Deviation function from excel
</commit_message>
<xml_diff>
--- a/AD-OCS/data/amoco_HN.xlsx
+++ b/AD-OCS/data/amoco_HN.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10560525_polimi_it/Documents/SUPER/PhD/Progetti Magistrali/Federico Rocca Thesis/Tecnologia/Data/Worksheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10619235_polimi_it/Documents/Documenti/GitHub/AD-OCS/AD-OCS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{854BF156-97D4-495F-9740-E4B6A28AF2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A796FF3-E402-4871-8804-37C51C9CB55A}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{854BF156-97D4-495F-9740-E4B6A28AF2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D6E9C3C-9015-42FC-BE31-611A2EE483C7}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="1620" windowWidth="14400" windowHeight="7270" firstSheet="1" activeTab="1" xr2:uid="{937B5A09-45AC-4F43-9144-B848BCA4D579}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{937B5A09-45AC-4F43-9144-B848BCA4D579}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_Values" sheetId="1" r:id="rId1"/>
     <sheet name="Influent" sheetId="2" r:id="rId2"/>
+    <sheet name="Deviations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>HRT
 [days]</t>
@@ -109,6 +110,9 @@
   <si>
     <t>Nin</t>
   </si>
+  <si>
+    <t>time</t>
+  </si>
 </sst>
 </file>
 
@@ -117,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +268,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -282,7 +286,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1495,23 +1499,23 @@
       <selection activeCell="O1" sqref="O1:O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7265625" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="43.5">
+    <row r="1" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1560,7 @@
       </c>
       <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>5</v>
       </c>
@@ -1601,7 +1605,7 @@
       </c>
       <c r="O2" s="15"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>8</v>
       </c>
@@ -1646,7 +1650,7 @@
       </c>
       <c r="O3" s="15"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>10</v>
       </c>
@@ -1691,7 +1695,7 @@
       </c>
       <c r="O4" s="15"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>12</v>
       </c>
@@ -1736,7 +1740,7 @@
       </c>
       <c r="O5" s="15"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>15</v>
       </c>
@@ -1781,7 +1785,7 @@
       </c>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>17</v>
       </c>
@@ -1826,7 +1830,7 @@
       </c>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="17">
         <v>20</v>
       </c>
@@ -1872,7 +1876,7 @@
       <c r="O8" s="21"/>
       <c r="P8" s="22"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>22</v>
       </c>
@@ -1917,7 +1921,7 @@
       </c>
       <c r="O9" s="15"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>25</v>
       </c>
@@ -1962,7 +1966,7 @@
       </c>
       <c r="O10" s="15"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>30</v>
       </c>
@@ -2007,7 +2011,7 @@
       </c>
       <c r="O11" s="15"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>50</v>
       </c>
@@ -2052,7 +2056,7 @@
       </c>
       <c r="O12" s="15"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>70</v>
       </c>
@@ -2097,7 +2101,7 @@
       </c>
       <c r="O13" s="15"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>90</v>
       </c>
@@ -2152,16 +2156,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3669712F-750D-47C9-80D6-49FB7FC94EF3}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2178,7 +2182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.2E-2</v>
       </c>
@@ -2193,6 +2197,98 @@
       </c>
       <c r="E2">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C458D2-0390-4007-98A4-66EBEC10F814}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>